<commit_message>
left forward and mips.v
</commit_message>
<xml_diff>
--- a/流水线设计.xlsx
+++ b/流水线设计.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D1D6E1-A96D-44FD-9227-94483F7B2D6E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD81F73-DAB5-460D-968B-D19BF225C51D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="145">
   <si>
     <t>部件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -378,22 +378,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cal_r/1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cal_i/1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>load/2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>load/1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>stall</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -438,14 +422,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FowardRsD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FowardRtD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GRF.RD1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -470,14 +446,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FowardRsE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FowardRtE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RD1E</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -498,10 +466,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FowardRtM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>WriteDataM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -594,7 +558,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>jal/0</t>
+    <t>NPC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cal_r/1rd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cal_i/1rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load/2rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jal/0ra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load/1rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForwardRsD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForwardRtD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForwardRsE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForwardRtE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForwardRtM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -660,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -676,6 +680,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -972,29 +979,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="10.21875" style="2" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="2"/>
+    <col min="2" max="2" width="10.19921875" style="2" customWidth="1"/>
+    <col min="3" max="5" width="9.1328125" style="1"/>
+    <col min="6" max="6" width="10.86328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="1" customWidth="1"/>
-    <col min="9" max="11" width="9.109375" style="1"/>
-    <col min="12" max="12" width="9.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="1"/>
-    <col min="15" max="15" width="9.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" style="1"/>
-    <col min="17" max="17" width="10.21875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.109375" style="1" customWidth="1"/>
+    <col min="9" max="11" width="9.1328125" style="1"/>
+    <col min="12" max="12" width="9.1328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1328125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.1328125" style="1"/>
+    <col min="15" max="15" width="9.86328125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1328125" style="1"/>
+    <col min="17" max="17" width="10.19921875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.1328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1027,7 @@
         <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>62</v>
@@ -1041,8 +1048,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1054,15 +1061,12 @@
       <c r="P2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="R2" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1103,8 +1107,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1145,8 +1149,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1185,12 +1189,12 @@
       </c>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>3</v>
@@ -1208,8 +1212,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
@@ -1250,11 +1254,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1288,9 +1292,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1304,7 +1308,7 @@
         <v>49</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>49</v>
@@ -1313,8 +1317,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1340,9 +1344,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1355,9 +1359,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1368,30 +1372,30 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="1" t="s">
         <v>63</v>
       </c>
@@ -1404,6 +1408,9 @@
       <c r="M14" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="N14" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="O14" s="1" t="s">
         <v>56</v>
       </c>
@@ -1411,8 +1418,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
@@ -1426,11 +1433,11 @@
         <v>64</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1458,8 +1465,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1473,14 +1480,14 @@
         <v>52</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1500,20 +1507,20 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
@@ -1551,11 +1558,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1580,21 +1587,21 @@
         <v>53</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>53</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1617,7 +1624,7 @@
         <v>22</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>23</v>
@@ -1626,14 +1633,14 @@
         <v>22</v>
       </c>
       <c r="Q22" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1658,14 +1665,14 @@
         <v>16</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A24" s="9"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1676,8 +1683,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1688,8 +1695,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
@@ -1727,11 +1734,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A27" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1747,9 +1754,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1760,8 +1767,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A29" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1774,8 +1781,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A30" s="9"/>
       <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
@@ -1798,8 +1805,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
@@ -1810,8 +1817,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1846,11 +1853,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1872,7 +1879,7 @@
         <v>72</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="M33" s="3">
         <v>31</v>
@@ -1890,9 +1897,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1912,7 +1919,7 @@
         <v>31</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="M34" s="3" t="s">
         <v>41</v>
@@ -1930,23 +1937,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B37" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
       <c r="I37" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B38" s="2" t="s">
         <v>79</v>
       </c>
@@ -1957,22 +1964,22 @@
         <v>78</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>90</v>
+        <v>136</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B39" s="2" t="s">
         <v>80</v>
       </c>
@@ -1983,19 +1990,19 @@
         <v>0</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B40" s="2" t="s">
         <v>82</v>
       </c>
@@ -2006,10 +2013,10 @@
         <v>1</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B41" s="2" t="s">
         <v>83</v>
       </c>
@@ -2020,10 +2027,10 @@
         <v>1</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B42" s="2" t="s">
         <v>85</v>
       </c>
@@ -2034,10 +2041,10 @@
         <v>1</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B43" s="2" t="s">
         <v>86</v>
       </c>
@@ -2048,12 +2055,12 @@
         <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B44" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>84</v>
@@ -2062,112 +2069,112 @@
         <v>0</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G46" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B47" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
       <c r="C48" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B49" s="2" t="s">
         <v>87</v>
       </c>
@@ -2175,82 +2182,78 @@
         <v>84</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="C50" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C50" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="E50" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="G50" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="I50" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B51" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
     <mergeCell ref="E37:H37"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A8:A15"/>
@@ -2264,6 +2267,10 @@
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
macro and first run in ISE
</commit_message>
<xml_diff>
--- a/流水线设计.xlsx
+++ b/流水线设计.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE4E0B9-2EDE-4E50-B730-E97A57F228E5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC6150A-0225-4EE8-80F2-DB53A599C3B8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -574,10 +574,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>jal/0ra</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>load/1rt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -599,6 +595,10 @@
   </si>
   <si>
     <t>ForwardRtM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>link/0ra</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -691,10 +691,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -979,29 +979,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="2"/>
-    <col min="2" max="2" width="10.19921875" style="2" customWidth="1"/>
-    <col min="3" max="5" width="9.1328125" style="1"/>
-    <col min="6" max="6" width="10.86328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.53125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="10.21875" style="2" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="1" customWidth="1"/>
-    <col min="9" max="11" width="9.1328125" style="1"/>
-    <col min="12" max="12" width="9.1328125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1328125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.1328125" style="1"/>
-    <col min="15" max="15" width="9.86328125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1328125" style="1"/>
-    <col min="17" max="17" width="10.19921875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1328125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="9.109375" style="1"/>
+    <col min="12" max="12" width="9.109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="1"/>
+    <col min="15" max="15" width="9.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="1"/>
+    <col min="17" max="17" width="10.21875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1048,8 +1048,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1065,8 +1065,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1107,8 +1107,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A4" s="10"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1149,8 +1149,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A5" s="10"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1189,8 +1189,8 @@
       </c>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1212,8 +1212,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A7" s="10"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
@@ -1254,11 +1254,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1292,9 +1292,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1317,8 +1317,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A10" s="10"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1344,9 +1344,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1359,9 +1359,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1372,9 +1372,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1393,9 +1393,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="1" t="s">
         <v>63</v>
       </c>
@@ -1418,8 +1418,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A15" s="10"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
@@ -1436,8 +1436,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1465,8 +1465,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A17" s="10"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1486,8 +1486,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A18" s="10"/>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1507,8 +1507,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A19" s="10"/>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
@@ -1519,8 +1519,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A20" s="10"/>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
@@ -1558,11 +1558,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1599,9 +1599,9 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1639,8 +1639,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1671,8 +1671,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A24" s="10"/>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1683,8 +1683,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A25" s="10"/>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1695,8 +1695,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A26" s="10"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
@@ -1734,11 +1734,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1754,9 +1754,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1767,8 +1767,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1781,8 +1781,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A30" s="10"/>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
       <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
@@ -1805,8 +1805,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A31" s="10"/>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
@@ -1817,8 +1817,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A32" s="10"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1853,11 +1853,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A33" s="10" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1897,9 +1897,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1937,23 +1937,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B37" s="10" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B37" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="9" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
       <c r="I37" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>79</v>
       </c>
@@ -1973,13 +1973,13 @@
         <v>137</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>80</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>82</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>83</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>85</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>86</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>90</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>91</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>94</v>
       </c>
@@ -2127,25 +2127,25 @@
         <v>98</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>95</v>
       </c>
@@ -2156,25 +2156,25 @@
         <v>99</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="K48" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J48" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="K48" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>87</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>104</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>106</v>
@@ -2197,13 +2197,13 @@
         <v>115</v>
       </c>
       <c r="I49" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J49" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>95</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>105</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>107</v>
@@ -2222,14 +2222,14 @@
       <c r="H50" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="I50" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J50" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J50" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>88</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>110</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>111</v>
@@ -2254,6 +2254,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="E37:H37"/>
     <mergeCell ref="A2:A5"/>
@@ -2269,8 +2271,6 @@
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
find question in forward
</commit_message>
<xml_diff>
--- a/流水线设计.xlsx
+++ b/流水线设计.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC6150A-0225-4EE8-80F2-DB53A599C3B8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FC8807-6E64-40DE-915A-89E06F40BDE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="146">
   <si>
     <t>部件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -599,6 +599,10 @@
   </si>
   <si>
     <t>link/0ra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不存在</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -643,12 +647,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -664,7 +674,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -694,6 +704,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -979,29 +992,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="10.21875" style="2" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="2"/>
+    <col min="2" max="2" width="10.19921875" style="2" customWidth="1"/>
+    <col min="3" max="5" width="9.1328125" style="1"/>
+    <col min="6" max="6" width="10.86328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="1" customWidth="1"/>
-    <col min="9" max="11" width="9.109375" style="1"/>
-    <col min="12" max="12" width="9.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="1"/>
-    <col min="15" max="15" width="9.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" style="1"/>
-    <col min="17" max="17" width="10.21875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.109375" style="1" customWidth="1"/>
+    <col min="9" max="11" width="9.1328125" style="1"/>
+    <col min="12" max="12" width="9.1328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1328125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.1328125" style="1"/>
+    <col min="15" max="15" width="9.86328125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1328125" style="1"/>
+    <col min="17" max="17" width="10.19921875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.1328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1061,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
@@ -1065,7 +1078,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -1107,7 +1120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -1149,7 +1162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>43</v>
@@ -1189,7 +1202,7 @@
       </c>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -1212,7 +1225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
         <v>25</v>
@@ -1254,7 +1267,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -1292,7 +1305,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="1" t="s">
@@ -1317,7 +1330,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -1344,7 +1357,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>10</v>
@@ -1359,7 +1372,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="1" t="s">
@@ -1372,7 +1385,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
         <v>13</v>
@@ -1393,7 +1406,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="1" t="s">
@@ -1418,7 +1431,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
         <v>43</v>
@@ -1436,7 +1449,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
@@ -1465,7 +1478,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -1486,7 +1499,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
         <v>22</v>
@@ -1507,7 +1520,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
         <v>39</v>
@@ -1519,7 +1532,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
         <v>40</v>
@@ -1558,7 +1571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
@@ -1599,7 +1612,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="1" t="s">
@@ -1639,7 +1652,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1671,7 +1684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A24" s="9"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
@@ -1683,7 +1696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
         <v>41</v>
@@ -1695,7 +1708,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
         <v>42</v>
@@ -1734,7 +1747,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A27" s="9" t="s">
         <v>29</v>
       </c>
@@ -1754,7 +1767,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
@@ -1767,7 +1780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1781,7 +1794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A30" s="9"/>
       <c r="B30" s="2" t="s">
         <v>31</v>
@@ -1805,7 +1818,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
         <v>37</v>
@@ -1817,7 +1830,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
         <v>38</v>
@@ -1853,7 +1866,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A33" s="9" t="s">
         <v>30</v>
       </c>
@@ -1897,7 +1910,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="1" t="s">
@@ -1937,7 +1950,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B37" s="9" t="s">
         <v>76</v>
       </c>
@@ -1953,7 +1966,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B38" s="2" t="s">
         <v>79</v>
       </c>
@@ -1979,7 +1992,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B39" s="2" t="s">
         <v>80</v>
       </c>
@@ -1998,11 +2011,14 @@
       <c r="G39" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="H39" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="I39" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B40" s="2" t="s">
         <v>82</v>
       </c>
@@ -2016,7 +2032,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B41" s="2" t="s">
         <v>83</v>
       </c>
@@ -2030,7 +2046,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B42" s="2" t="s">
         <v>85</v>
       </c>
@@ -2044,7 +2060,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B43" s="2" t="s">
         <v>86</v>
       </c>
@@ -2058,7 +2074,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B44" s="2" t="s">
         <v>90</v>
       </c>
@@ -2077,11 +2093,14 @@
       <c r="G44" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="H44" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="I44" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B46" s="2" t="s">
         <v>91</v>
       </c>
@@ -2109,11 +2128,11 @@
       <c r="J46" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="K46" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B47" s="2" t="s">
         <v>94</v>
       </c>
@@ -2132,7 +2151,7 @@
       <c r="G47" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="11" t="s">
         <v>130</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -2141,11 +2160,11 @@
       <c r="J47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="K47" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
       <c r="C48" s="1" t="s">
         <v>95</v>
       </c>
@@ -2161,7 +2180,7 @@
       <c r="G48" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H48" s="7" t="s">
+      <c r="H48" s="11" t="s">
         <v>130</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -2170,11 +2189,11 @@
       <c r="J48" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="K48" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B49" s="2" t="s">
         <v>87</v>
       </c>
@@ -2199,11 +2218,11 @@
       <c r="I49" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="J49" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.4">
       <c r="C50" s="1" t="s">
         <v>95</v>
       </c>
@@ -2225,11 +2244,11 @@
       <c r="I50" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="J50" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B51" s="2" t="s">
         <v>88</v>
       </c>
@@ -2248,12 +2267,13 @@
       <c r="G51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H51" s="11" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B11:B12"/>
@@ -2270,7 +2290,6 @@
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
delete the WBWB to ID forward
</commit_message>
<xml_diff>
--- a/流水线设计.xlsx
+++ b/流水线设计.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FC8807-6E64-40DE-915A-89E06F40BDE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF725CB-0DEC-4368-87D4-2EB14D6753E3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="145">
   <si>
     <t>部件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -551,10 +551,6 @@
   </si>
   <si>
     <t>输入3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>输入4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -674,7 +670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,13 +696,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -993,28 +995,28 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="2"/>
-    <col min="2" max="2" width="10.19921875" style="2" customWidth="1"/>
-    <col min="3" max="5" width="9.1328125" style="1"/>
-    <col min="6" max="6" width="10.86328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.53125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="10.21875" style="2" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="1" customWidth="1"/>
-    <col min="9" max="11" width="9.1328125" style="1"/>
-    <col min="12" max="12" width="9.1328125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1328125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.1328125" style="1"/>
-    <col min="15" max="15" width="9.86328125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1328125" style="1"/>
-    <col min="17" max="17" width="10.19921875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1328125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="9.109375" style="1"/>
+    <col min="12" max="12" width="9.109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="1"/>
+    <col min="15" max="15" width="9.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="1"/>
+    <col min="17" max="17" width="10.21875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1061,8 +1063,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1078,8 +1080,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" s="9"/>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1120,8 +1122,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A4" s="9"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1162,8 +1164,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A5" s="9"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1202,8 +1204,8 @@
       </c>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1225,8 +1227,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
@@ -1267,11 +1269,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1305,9 +1307,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1330,8 +1332,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A10" s="9"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1357,9 +1359,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1372,9 +1374,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1385,9 +1387,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1406,9 +1408,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="1" t="s">
         <v>63</v>
       </c>
@@ -1431,8 +1433,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A15" s="9"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
@@ -1446,11 +1448,11 @@
         <v>64</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A16" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1478,8 +1480,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A17" s="9"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1499,8 +1501,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A18" s="9"/>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
       <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1520,8 +1522,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A19" s="9"/>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
@@ -1532,8 +1534,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A20" s="9"/>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
@@ -1571,11 +1573,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1612,9 +1614,9 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1652,8 +1654,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1684,8 +1686,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A24" s="9"/>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1696,8 +1698,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A25" s="9"/>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1708,8 +1710,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A26" s="9"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
@@ -1747,11 +1749,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1767,9 +1769,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1780,8 +1782,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A29" s="9" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1794,8 +1796,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A30" s="9"/>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
       <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
@@ -1818,8 +1820,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A31" s="9"/>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
       <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
@@ -1830,8 +1832,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A32" s="9"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
       <c r="B32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1866,11 +1868,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1910,9 +1912,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1950,23 +1952,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B37" s="9" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B37" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="10" t="s">
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
       <c r="I37" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>79</v>
       </c>
@@ -1977,22 +1979,22 @@
         <v>78</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>80</v>
       </c>
@@ -2012,13 +2014,13 @@
         <v>89</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>82</v>
       </c>
@@ -2032,7 +2034,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>83</v>
       </c>
@@ -2046,7 +2048,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>85</v>
       </c>
@@ -2060,7 +2062,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>86</v>
       </c>
@@ -2074,7 +2076,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>90</v>
       </c>
@@ -2094,13 +2096,13 @@
         <v>89</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>91</v>
       </c>
@@ -2128,11 +2130,9 @@
       <c r="J46" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="K46" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="K46" s="12"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>94</v>
       </c>
@@ -2146,12 +2146,12 @@
         <v>98</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="9" t="s">
         <v>130</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -2160,11 +2160,9 @@
       <c r="J47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="K47" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="K47" s="12"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>95</v>
       </c>
@@ -2175,12 +2173,12 @@
         <v>99</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H48" s="9" t="s">
         <v>130</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -2189,11 +2187,9 @@
       <c r="J48" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="K48" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="K48" s="12"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>87</v>
       </c>
@@ -2207,7 +2203,7 @@
         <v>104</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>106</v>
@@ -2218,11 +2214,11 @@
       <c r="I49" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J49" s="11" t="s">
+      <c r="J49" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>95</v>
       </c>
@@ -2233,7 +2229,7 @@
         <v>105</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>107</v>
@@ -2244,11 +2240,11 @@
       <c r="I50" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="J50" s="11" t="s">
+      <c r="J50" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>88</v>
       </c>
@@ -2262,22 +2258,18 @@
         <v>110</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="H51" s="13" t="s">
         <v>116</v>
       </c>
+      <c r="J51" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="E37:H37"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A8:A15"/>
     <mergeCell ref="B37:D37"/>
@@ -2290,6 +2282,11 @@
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="E37:H37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish the thinking question
</commit_message>
<xml_diff>
--- a/流水线设计.xlsx
+++ b/流水线设计.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8A869B-B502-4B6D-83F9-831747D85FDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB419BF-E015-430C-B630-EAA2584A1F16}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="155">
   <si>
     <t>部件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -619,6 +619,26 @@
   </si>
   <si>
     <t>采用GRF内部转发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEMtoEX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WBtoEX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEMtoID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WBtoMEM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -684,7 +704,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -716,10 +736,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1003,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="B29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1075,7 +1098,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1092,7 +1115,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1134,7 +1157,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1176,7 +1199,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1216,7 +1239,7 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1239,7 +1262,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
@@ -1281,10 +1304,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1319,8 +1342,8 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1344,7 +1367,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1371,8 +1394,8 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1386,8 +1409,8 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1399,8 +1422,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1420,8 +1443,8 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="1" t="s">
         <v>63</v>
       </c>
@@ -1445,7 +1468,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
@@ -1463,7 +1486,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1492,7 +1515,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1513,7 +1536,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1534,7 +1557,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
@@ -1546,7 +1569,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
@@ -1585,10 +1608,10 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1626,8 +1649,8 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1666,7 +1689,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1698,7 +1721,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1710,7 +1733,7 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1722,7 +1745,7 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
@@ -1761,10 +1784,10 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1781,8 +1804,8 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1794,7 +1817,7 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1808,7 +1831,7 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A30" s="11"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
@@ -1832,7 +1855,7 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
@@ -1844,7 +1867,7 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1880,10 +1903,10 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1924,8 +1947,8 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1964,29 +1987,29 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="10" t="s">
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10" t="s">
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="11" t="s">
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B38" s="2" t="s">
@@ -2057,15 +2080,24 @@
       <c r="H39" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="I39" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>152</v>
+      </c>
       <c r="K39" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M39" s="11" t="s">
+      <c r="L39" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="M39" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B40" s="2" t="s">
@@ -2077,15 +2109,34 @@
       <c r="D40" s="1">
         <v>1</v>
       </c>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
+      <c r="E40" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>150</v>
+      </c>
       <c r="G40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
+      <c r="H40" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K40" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="L40" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="12"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B41" s="2" t="s">
@@ -2097,15 +2148,34 @@
       <c r="D41" s="1">
         <v>1</v>
       </c>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
+      <c r="E41" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>150</v>
+      </c>
       <c r="G41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
+      <c r="H41" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K41" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="L41" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B42" s="2" t="s">
@@ -2117,15 +2187,34 @@
       <c r="D42" s="1">
         <v>1</v>
       </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
+      <c r="E42" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>150</v>
+      </c>
       <c r="G42" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
+      <c r="H42" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B43" s="2" t="s">
@@ -2137,15 +2226,34 @@
       <c r="D43" s="1">
         <v>1</v>
       </c>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
+      <c r="E43" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>150</v>
+      </c>
       <c r="G43" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
+      <c r="H43" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K43" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="L43" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+      <c r="P43" s="12"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B44" s="2" t="s">
@@ -2169,188 +2277,232 @@
       <c r="H44" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="I44" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>152</v>
+      </c>
       <c r="K44" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
+      <c r="L44" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B45" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L45" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="K46" s="12"/>
+      <c r="K46" s="11"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K47" s="11"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B48" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H47" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K47" s="12"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="C48" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H48" s="12" t="s">
+      <c r="H48" s="11" t="s">
         <v>130</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J48" s="7" t="s">
+      <c r="J48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="K48" s="12"/>
+      <c r="K48" s="11"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B50" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="J49" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="C50" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="I50" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J50" s="12" t="s">
+      <c r="J50" s="11" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B51" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="C51" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J51" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B52" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H51" s="12" t="s">
+      <c r="H52" s="11" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="I37:L37"/>
     <mergeCell ref="M37:P37"/>
-    <mergeCell ref="M39:P44"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A8:A15"/>
     <mergeCell ref="B37:D37"/>
@@ -2364,6 +2516,12 @@
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="M39:P45"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="I37:L37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
delete the PC8E to ID
</commit_message>
<xml_diff>
--- a/流水线设计.xlsx
+++ b/流水线设计.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB419BF-E015-430C-B630-EAA2584A1F16}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1A7A1E-6526-45AA-94DD-2F80AAC8EC4D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="154">
   <si>
     <t>部件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -539,10 +539,6 @@
   </si>
   <si>
     <t>ALUOutW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC8E</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1028,29 +1024,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:J52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="2"/>
-    <col min="2" max="2" width="10.19921875" style="2" customWidth="1"/>
-    <col min="3" max="5" width="9.1328125" style="1"/>
-    <col min="6" max="6" width="10.86328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.53125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="10.21875" style="2" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="1" customWidth="1"/>
-    <col min="9" max="11" width="9.1328125" style="1"/>
-    <col min="12" max="12" width="9.1328125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1328125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.1328125" style="1"/>
-    <col min="15" max="15" width="9.86328125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1328125" style="1"/>
-    <col min="17" max="17" width="10.19921875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1328125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="9.109375" style="1"/>
+    <col min="12" max="12" width="9.109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="1"/>
+    <col min="15" max="15" width="9.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="1"/>
+    <col min="17" max="17" width="10.21875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1093,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>44</v>
       </c>
@@ -1114,7 +1110,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -1156,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -1198,7 +1194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>43</v>
@@ -1238,7 +1234,7 @@
       </c>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -1261,7 +1257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="5" t="s">
         <v>25</v>
@@ -1303,7 +1299,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>14</v>
       </c>
@@ -1341,7 +1337,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="1" t="s">
@@ -1366,7 +1362,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -1393,7 +1389,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12" t="s">
         <v>10</v>
@@ -1408,7 +1404,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="1" t="s">
@@ -1421,7 +1417,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12" t="s">
         <v>13</v>
@@ -1442,7 +1438,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="1" t="s">
@@ -1467,7 +1463,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
         <v>43</v>
@@ -1482,10 +1478,10 @@
         <v>64</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
@@ -1514,7 +1510,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -1535,7 +1531,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="2" t="s">
         <v>22</v>
@@ -1556,7 +1552,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="2" t="s">
         <v>39</v>
@@ -1568,7 +1564,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="2" t="s">
         <v>40</v>
@@ -1607,7 +1603,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
@@ -1648,7 +1644,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="1" t="s">
@@ -1688,7 +1684,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>26</v>
       </c>
@@ -1720,7 +1716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
@@ -1732,7 +1728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="2" t="s">
         <v>41</v>
@@ -1744,7 +1740,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="2" t="s">
         <v>42</v>
@@ -1783,7 +1779,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>29</v>
       </c>
@@ -1803,7 +1799,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="1" t="s">
@@ -1816,7 +1812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>32</v>
       </c>
@@ -1830,7 +1826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="2" t="s">
         <v>31</v>
@@ -1854,7 +1850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="2" t="s">
         <v>37</v>
@@ -1866,7 +1862,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="2" t="s">
         <v>38</v>
@@ -1902,7 +1898,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>30</v>
       </c>
@@ -1946,7 +1942,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="1" t="s">
@@ -1986,7 +1982,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B37" s="12" t="s">
         <v>76</v>
       </c>
@@ -2005,13 +2001,13 @@
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
       <c r="M37" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N37" s="12"/>
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>79</v>
       </c>
@@ -2022,43 +2018,43 @@
         <v>78</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="I38" s="1" t="s">
+      <c r="L38" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="N38" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="O38" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="P38" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="M38" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="N38" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="O38" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="P38" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>80</v>
       </c>
@@ -2078,28 +2074,28 @@
         <v>89</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>89</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M39" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N39" s="12"/>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>82</v>
       </c>
@@ -2110,35 +2106,35 @@
         <v>1</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H40" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="I40" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="I40" s="10" t="s">
-        <v>151</v>
-      </c>
       <c r="J40" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
       <c r="O40" s="12"/>
       <c r="P40" s="12"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>83</v>
       </c>
@@ -2149,35 +2145,35 @@
         <v>1</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H41" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="I41" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="I41" s="10" t="s">
-        <v>151</v>
-      </c>
       <c r="J41" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M41" s="12"/>
       <c r="N41" s="12"/>
       <c r="O41" s="12"/>
       <c r="P41" s="12"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>85</v>
       </c>
@@ -2188,35 +2184,35 @@
         <v>1</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H42" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="I42" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="I42" s="10" t="s">
-        <v>151</v>
-      </c>
       <c r="J42" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
       <c r="O42" s="12"/>
       <c r="P42" s="12"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>86</v>
       </c>
@@ -2227,35 +2223,35 @@
         <v>1</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H43" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="I43" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="I43" s="10" t="s">
-        <v>151</v>
-      </c>
       <c r="J43" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L43" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M43" s="12"/>
       <c r="N43" s="12"/>
       <c r="O43" s="12"/>
       <c r="P43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>90</v>
       </c>
@@ -2275,68 +2271,68 @@
         <v>89</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>89</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D45" s="1">
         <v>2</v>
       </c>
       <c r="E45" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F45" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="J45" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="L45" s="10" t="s">
-        <v>152</v>
       </c>
       <c r="M45" s="12"/>
       <c r="N45" s="12"/>
       <c r="O45" s="12"/>
       <c r="P45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>91</v>
       </c>
@@ -2362,11 +2358,11 @@
         <v>114</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2380,23 +2376,19 @@
         <v>98</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K48" s="11"/>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>95</v>
       </c>
@@ -2407,22 +2399,19 @@
         <v>99</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="H49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I49" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="I49" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="J49" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>87</v>
       </c>
@@ -2436,7 +2425,7 @@
         <v>104</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>106</v>
@@ -2445,13 +2434,13 @@
         <v>115</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>95</v>
       </c>
@@ -2462,7 +2451,7 @@
         <v>105</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>107</v>
@@ -2471,13 +2460,13 @@
         <v>115</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J51" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>88</v>
       </c>
@@ -2491,7 +2480,7 @@
         <v>110</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>111</v>
@@ -2502,6 +2491,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="M39:P45"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="I37:L37"/>
     <mergeCell ref="M37:P37"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A8:A15"/>
@@ -2516,12 +2511,6 @@
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="M39:P45"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="I37:L37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>